<commit_message>
removed csv and updated av_issues.xlsx to remove unneccessary dates
</commit_message>
<xml_diff>
--- a/src/av_issues.xlsx
+++ b/src/av_issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\circ8\Documents\Chris\GitHub Repositories\library-av-app\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12559FD-B22A-4F45-9B2B-02048A3CA84D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED65F9CE-0F1A-4FFD-92E5-7D715AB8EC68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16950" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1455,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3181,46 +3181,6 @@
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>45652</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>45652</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>45652</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>45652</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
-        <v>45652</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>45652</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>45652</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>45652</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="2833" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>